<commit_message>
Bulk of schematic work finished, beginning layout
</commit_message>
<xml_diff>
--- a/Documentation/RevC Documents/RevC_PowerCalculations.xlsx
+++ b/Documentation/RevC Documents/RevC_PowerCalculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12270"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Rev C dc-dc psu requirements</t>
   </si>
@@ -174,6 +174,27 @@
   </si>
   <si>
     <t xml:space="preserve">LCD and LEDs on </t>
+  </si>
+  <si>
+    <t>Results:</t>
+  </si>
+  <si>
+    <t>Pout</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Efficiency </t>
+  </si>
+  <si>
+    <t>Current In Max @ 18v</t>
+  </si>
+  <si>
+    <t>Current In Max @ 50v</t>
   </si>
 </sst>
 </file>
@@ -246,18 +267,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,15 +559,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -562,59 +583,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="4" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="R2" s="4" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="R2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -629,23 +650,23 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -778,7 +799,7 @@
       <c r="K6">
         <v>60</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="O6">
@@ -837,6 +858,18 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
       <c r="J8" t="s">
         <v>22</v>
       </c>
@@ -861,11 +894,6 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>49</v>
@@ -888,6 +916,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="R12" t="s">
         <v>42</v>
       </c>
@@ -897,6 +928,47 @@
       </c>
       <c r="T12" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1">
+        <f>C7/1000*C4</f>
+        <v>3.2594759999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B13*(1/C8)*100</f>
+        <v>4.0743450000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="1">
+        <f>B14/18</f>
+        <v>0.22635250000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1">
+        <f>B14/50</f>
+        <v>8.1486900000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>